<commit_message>
add plotting predicted hospitals on saarland map
</commit_message>
<xml_diff>
--- a/src/index_travel_accessibility/data/processed/calculated_metrics_from_travel_time.xlsx
+++ b/src/index_travel_accessibility/data/processed/calculated_metrics_from_travel_time.xlsx
@@ -477,19 +477,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17.466</v>
+        <v>17.812</v>
       </c>
       <c r="C2" t="n">
-        <v>12.08</v>
+        <v>12.66</v>
       </c>
       <c r="D2" t="n">
-        <v>28.85</v>
+        <v>29.056</v>
       </c>
       <c r="E2" t="n">
-        <v>0.771978021978022</v>
+        <v>0.8247863247863249</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2857142857142857</v>
+        <v>0.3381555153707053</v>
       </c>
       <c r="G2" t="n">
         <v>1</v>
@@ -542,7 +542,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.4064773527340999</v>
+        <v>0.3968835930339138</v>
       </c>
     </row>
     <row r="5">
@@ -567,7 +567,7 @@
         <v>0.6112115732368897</v>
       </c>
       <c r="G5" t="n">
-        <v>0.7873738559023705</v>
+        <v>0.7687901008249315</v>
       </c>
     </row>
     <row r="6">
@@ -592,7 +592,7 @@
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.5817883126026757</v>
+        <v>0.5680568285976172</v>
       </c>
     </row>
     <row r="7">
@@ -617,7 +617,7 @@
         <v>0.7992766726943943</v>
       </c>
       <c r="G7" t="n">
-        <v>0.4832199014315892</v>
+        <v>0.4718148487626035</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update hospital capacity index to convert index into numeric
</commit_message>
<xml_diff>
--- a/src/index_travel_accessibility/data/processed/calculated_metrics_from_travel_time.xlsx
+++ b/src/index_travel_accessibility/data/processed/calculated_metrics_from_travel_time.xlsx
@@ -486,10 +486,10 @@
         <v>29.056</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8247863247863249</v>
+        <v>0.8220155038759691</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3381555153707053</v>
+        <v>0.3061611374407583</v>
       </c>
       <c r="G2" t="n">
         <v>1</v>
@@ -511,10 +511,10 @@
         <v>20.328</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5515873015873013</v>
+        <v>0.5444961240310074</v>
       </c>
       <c r="F3" t="n">
-        <v>0.7721518987341772</v>
+        <v>0.7611374407582939</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -527,10 +527,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>12.408</v>
+        <v>12.51</v>
       </c>
       <c r="C4" t="n">
-        <v>8.92</v>
+        <v>9.43</v>
       </c>
       <c r="D4" t="n">
         <v>23.792</v>
@@ -561,10 +561,10 @@
         <v>27.038</v>
       </c>
       <c r="E5" t="n">
-        <v>0.7118437118437116</v>
+        <v>0.7072868217054261</v>
       </c>
       <c r="F5" t="n">
-        <v>0.6112115732368897</v>
+        <v>0.5924170616113744</v>
       </c>
       <c r="G5" t="n">
         <v>0.7687901008249315</v>
@@ -611,10 +611,10 @@
         <v>24.446</v>
       </c>
       <c r="E7" t="n">
-        <v>0.996031746031746</v>
+        <v>0.995968992248062</v>
       </c>
       <c r="F7" t="n">
-        <v>0.7992766726943943</v>
+        <v>0.78957345971564</v>
       </c>
       <c r="G7" t="n">
         <v>0.4718148487626035</v>

</xml_diff>

<commit_message>
add bed allocation, update planner
</commit_message>
<xml_diff>
--- a/src/index_travel_accessibility/data/processed/calculated_metrics_from_travel_time.xlsx
+++ b/src/index_travel_accessibility/data/processed/calculated_metrics_from_travel_time.xlsx
@@ -477,19 +477,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17.812</v>
+        <v>17.466</v>
       </c>
       <c r="C2" t="n">
-        <v>12.66</v>
+        <v>12.08</v>
       </c>
       <c r="D2" t="n">
-        <v>29.056</v>
+        <v>28.85</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8220155038759691</v>
+        <v>0.7682283586720448</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3061611374407583</v>
+        <v>0.2511848341232228</v>
       </c>
       <c r="G2" t="n">
         <v>1</v>
@@ -511,7 +511,7 @@
         <v>20.328</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5444961240310074</v>
+        <v>0.5442134657151719</v>
       </c>
       <c r="F3" t="n">
         <v>0.7611374407582939</v>
@@ -527,7 +527,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>12.51</v>
+        <v>12.514</v>
       </c>
       <c r="C4" t="n">
         <v>9.43</v>
@@ -542,7 +542,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.3968835930339138</v>
+        <v>0.4064773527340999</v>
       </c>
     </row>
     <row r="5">
@@ -561,13 +561,13 @@
         <v>27.038</v>
       </c>
       <c r="E5" t="n">
-        <v>0.7072868217054261</v>
+        <v>0.7071051815079117</v>
       </c>
       <c r="F5" t="n">
         <v>0.5924170616113744</v>
       </c>
       <c r="G5" t="n">
-        <v>0.7687901008249315</v>
+        <v>0.7873738559023705</v>
       </c>
     </row>
     <row r="6">
@@ -592,7 +592,7 @@
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.5680568285976172</v>
+        <v>0.5817883126026757</v>
       </c>
     </row>
     <row r="7">
@@ -611,13 +611,13 @@
         <v>24.446</v>
       </c>
       <c r="E7" t="n">
-        <v>0.995968992248062</v>
+        <v>0.9959664908470369</v>
       </c>
       <c r="F7" t="n">
         <v>0.78957345971564</v>
       </c>
       <c r="G7" t="n">
-        <v>0.4718148487626035</v>
+        <v>0.4832199014315892</v>
       </c>
     </row>
   </sheetData>

</xml_diff>